<commit_message>
added view iamges script
</commit_message>
<xml_diff>
--- a/accuracy_scores.xlsx
+++ b/accuracy_scores.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,6 +447,149 @@
         <is>
           <t>Segment Gen</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Crypto_website</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>95</v>
+      </c>
+      <c r="C2" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Figma_food_website</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>80</v>
+      </c>
+      <c r="C3" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hyer_website</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>85</v>
+      </c>
+      <c r="C4" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>JoeCoffee-website-february-2022</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>78</v>
+      </c>
+      <c r="C5" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>mubasic_website</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>95</v>
+      </c>
+      <c r="C6" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>overflow_website</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>87</v>
+      </c>
+      <c r="C7" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>RCA_website</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>60</v>
+      </c>
+      <c r="C8" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Spotify_website</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>60</v>
+      </c>
+      <c r="C9" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Superlist_website</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>83</v>
+      </c>
+      <c r="C10" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Trees_website</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>83</v>
+      </c>
+      <c r="C11" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>webflow-full</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>72</v>
+      </c>
+      <c r="C12" t="n">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -460,7 +603,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +622,149 @@
         <is>
           <t>Segment Gen</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Crypto_website</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>95</v>
+      </c>
+      <c r="C2" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Figma_food_website</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>75</v>
+      </c>
+      <c r="C3" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hyer_website</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>80</v>
+      </c>
+      <c r="C4" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>JoeCoffee-website-february-2022</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>75</v>
+      </c>
+      <c r="C5" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>mubasic_website</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>95</v>
+      </c>
+      <c r="C6" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>overflow_website</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>85</v>
+      </c>
+      <c r="C7" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>RCA_website</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>70</v>
+      </c>
+      <c r="C8" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Spotify_website</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>70</v>
+      </c>
+      <c r="C9" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Superlist_website</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>85</v>
+      </c>
+      <c r="C10" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Trees_website</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>85</v>
+      </c>
+      <c r="C11" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>webflow-full</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>85</v>
+      </c>
+      <c r="C12" t="n">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -492,7 +778,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,6 +797,149 @@
         <is>
           <t>Segment Gen</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Crypto_website</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C2" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Figma_food_website</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>90</v>
+      </c>
+      <c r="C3" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hyer_website</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>90</v>
+      </c>
+      <c r="C4" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>JoeCoffee-website-february-2022</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>90</v>
+      </c>
+      <c r="C5" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>mubasic_website</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>100</v>
+      </c>
+      <c r="C6" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>overflow_website</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>95</v>
+      </c>
+      <c r="C7" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>RCA_website</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>60</v>
+      </c>
+      <c r="C8" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Spotify_website</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>60</v>
+      </c>
+      <c r="C9" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Superlist_website</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>90</v>
+      </c>
+      <c r="C10" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Trees_website</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>95</v>
+      </c>
+      <c r="C11" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>webflow-full</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>60</v>
+      </c>
+      <c r="C12" t="n">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -524,7 +953,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,6 +974,149 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Crypto_website</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>90</v>
+      </c>
+      <c r="C2" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Figma_food_website</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>85</v>
+      </c>
+      <c r="C3" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hyer_website</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>85</v>
+      </c>
+      <c r="C4" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>JoeCoffee-website-february-2022</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>70</v>
+      </c>
+      <c r="C5" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>mubasic_website</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>90</v>
+      </c>
+      <c r="C6" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>overflow_website</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>80</v>
+      </c>
+      <c r="C7" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>RCA_website</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>50</v>
+      </c>
+      <c r="C8" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Spotify_website</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>50</v>
+      </c>
+      <c r="C9" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Superlist_website</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>75</v>
+      </c>
+      <c r="C10" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Trees_website</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>70</v>
+      </c>
+      <c r="C11" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>webflow-full</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>70</v>
+      </c>
+      <c r="C12" t="n">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
setup accuracy score logging
</commit_message>
<xml_diff>
--- a/accuracy_scores.xlsx
+++ b/accuracy_scores.xlsx
@@ -452,115 +452,115 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Crypto_website</t>
+          <t>Figma_food_website</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="C2" t="n">
-        <v>90</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Figma_food_website</t>
+          <t>Trees_website</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="C3" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Hyer_website</t>
+          <t>JoeCoffee-website-february-2022</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C4" t="n">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>JoeCoffee-website-february-2022</t>
+          <t>Hyer_website</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C5" t="n">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>mubasic_website</t>
+          <t>webflow-full</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="C6" t="n">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>overflow_website</t>
+          <t>Superlist_website</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C7" t="n">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>RCA_website</t>
+          <t>Spotify_website</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C8" t="n">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Spotify_website</t>
+          <t>mubasic_website</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="C9" t="n">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Superlist_website</t>
+          <t>overflow_website</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C10" t="n">
         <v>87</v>
@@ -569,27 +569,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Trees_website</t>
+          <t>RCA_website</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C11" t="n">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>webflow-full</t>
+          <t>Crypto_website</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C12" t="n">
-        <v>73</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -627,50 +627,50 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Crypto_website</t>
+          <t>Figma_food_website</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="C2" t="n">
-        <v>90</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Figma_food_website</t>
+          <t>Trees_website</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="C3" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Hyer_website</t>
+          <t>JoeCoffee-website-february-2022</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C4" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>JoeCoffee-website-february-2022</t>
+          <t>Hyer_website</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C5" t="n">
         <v>85</v>
@@ -679,20 +679,20 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>mubasic_website</t>
+          <t>webflow-full</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C6" t="n">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>overflow_website</t>
+          <t>Superlist_website</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -705,7 +705,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>RCA_website</t>
+          <t>Spotify_website</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -718,20 +718,20 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Spotify_website</t>
+          <t>mubasic_website</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="C9" t="n">
-        <v>70</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Superlist_website</t>
+          <t>overflow_website</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -744,27 +744,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Trees_website</t>
+          <t>RCA_website</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="C11" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>webflow-full</t>
+          <t>Crypto_website</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>85</v>
       </c>
       <c r="C12" t="n">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -802,46 +802,46 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Crypto_website</t>
+          <t>Figma_food_website</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Figma_food_website</t>
+          <t>Trees_website</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>90</v>
       </c>
       <c r="C3" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Hyer_website</t>
+          <t>JoeCoffee-website-february-2022</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>90</v>
       </c>
       <c r="C4" t="n">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>JoeCoffee-website-february-2022</t>
+          <t>Hyer_website</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -854,50 +854,50 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>mubasic_website</t>
+          <t>webflow-full</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="C6" t="n">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>overflow_website</t>
+          <t>Superlist_website</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C7" t="n">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>RCA_website</t>
+          <t>Spotify_website</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C8" t="n">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Spotify_website</t>
+          <t>mubasic_website</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="C9" t="n">
         <v>90</v>
@@ -906,11 +906,11 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Superlist_website</t>
+          <t>overflow_website</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C10" t="n">
         <v>95</v>
@@ -919,27 +919,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Trees_website</t>
+          <t>RCA_website</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="C11" t="n">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>webflow-full</t>
+          <t>Crypto_website</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C12" t="n">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -977,72 +977,72 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Crypto_website</t>
+          <t>Figma_food_website</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="C2" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Figma_food_website</t>
+          <t>Trees_website</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="C3" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Hyer_website</t>
+          <t>JoeCoffee-website-february-2022</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C4" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>JoeCoffee-website-february-2022</t>
+          <t>Hyer_website</t>
         </is>
       </c>
       <c r="B5" t="n">
+        <v>80</v>
+      </c>
+      <c r="C5" t="n">
         <v>70</v>
-      </c>
-      <c r="C5" t="n">
-        <v>80</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>mubasic_website</t>
+          <t>webflow-full</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="C6" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>overflow_website</t>
+          <t>Superlist_website</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1055,37 +1055,37 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>RCA_website</t>
+          <t>Spotify_website</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C8" t="n">
-        <v>75</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Spotify_website</t>
+          <t>mubasic_website</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C9" t="n">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Superlist_website</t>
+          <t>overflow_website</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C10" t="n">
         <v>80</v>
@@ -1094,11 +1094,11 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Trees_website</t>
+          <t>RCA_website</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="C11" t="n">
         <v>60</v>
@@ -1107,14 +1107,14 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>webflow-full</t>
+          <t>Crypto_website</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C12" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited prompts and reran tests
</commit_message>
<xml_diff>
--- a/accuracy_scores.xlsx
+++ b/accuracy_scores.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,7 +437,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr"/>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Image Name</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Full Image Gen</t>
@@ -448,6 +452,7 @@
           <t>Segment Gen</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -456,11 +461,12 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>77</v>
+        <v>40</v>
       </c>
       <c r="C2" t="n">
-        <v>75</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -469,11 +475,12 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="C3" t="n">
-        <v>73</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -482,11 +489,12 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="C4" t="n">
-        <v>83</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -498,98 +506,162 @@
         <v>80</v>
       </c>
       <c r="C5" t="n">
-        <v>83</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>webflow-full</t>
+          <t>ecommerce</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="C6" t="n">
-        <v>80</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Superlist_website</t>
+          <t>webflow-full</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C7" t="n">
-        <v>85</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Spotify_website</t>
+          <t>complex</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C8" t="n">
-        <v>75</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>mubasic_website</t>
+          <t>Superlist_website</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C9" t="n">
-        <v>83</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>overflow_website</t>
+          <t>Spotify_website</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C10" t="n">
-        <v>87</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>RCA_website</t>
+          <t>blog</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="C11" t="n">
-        <v>72</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>mubasic_website</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>95</v>
+      </c>
+      <c r="C12" t="n">
+        <v>87</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>overflow_website</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>87</v>
+      </c>
+      <c r="C13" t="n">
+        <v>83</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>RCA_website</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>30</v>
+      </c>
+      <c r="C14" t="n">
+        <v>60</v>
+      </c>
+      <c r="D14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>Crypto_website</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>90</v>
-      </c>
-      <c r="C12" t="n">
-        <v>95</v>
+      <c r="B15" t="n">
+        <v>87</v>
+      </c>
+      <c r="C15" t="n">
+        <v>95</v>
+      </c>
+      <c r="D15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="n">
+        <v>87</v>
+      </c>
+      <c r="C16" t="n">
+        <v>92</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Crypto_website</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -603,7 +675,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -612,7 +684,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr"/>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Image Name</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Full Image Gen</t>
@@ -623,6 +699,7 @@
           <t>Segment Gen</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -631,11 +708,12 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C2" t="n">
-        <v>75</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -644,11 +722,12 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C3" t="n">
         <v>60</v>
       </c>
+      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -657,11 +736,12 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C4" t="n">
-        <v>90</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -670,55 +750,59 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C5" t="n">
-        <v>85</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>webflow-full</t>
+          <t>ecommerce</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="C6" t="n">
-        <v>80</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Superlist_website</t>
+          <t>webflow-full</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C7" t="n">
-        <v>85</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Spotify_website</t>
+          <t>complex</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C8" t="n">
-        <v>70</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>mubasic_website</t>
+          <t>Superlist_website</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -727,44 +811,104 @@
       <c r="C9" t="n">
         <v>85</v>
       </c>
+      <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>overflow_website</t>
+          <t>Spotify_website</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C10" t="n">
-        <v>85</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>RCA_website</t>
+          <t>blog</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>70</v>
+        <v>95</v>
       </c>
       <c r="C11" t="n">
-        <v>70</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>mubasic_website</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>95</v>
+      </c>
+      <c r="C12" t="n">
+        <v>80</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>overflow_website</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>85</v>
+      </c>
+      <c r="C13" t="n">
+        <v>85</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>RCA_website</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>40</v>
+      </c>
+      <c r="C14" t="n">
+        <v>60</v>
+      </c>
+      <c r="D14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>Crypto_website</t>
         </is>
       </c>
-      <c r="B12" t="n">
+      <c r="B15" t="n">
         <v>85</v>
       </c>
-      <c r="C12" t="n">
-        <v>95</v>
+      <c r="C15" t="n">
+        <v>95</v>
+      </c>
+      <c r="D15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="n">
+        <v>85</v>
+      </c>
+      <c r="C16" t="n">
+        <v>95</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Crypto_website</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -778,7 +922,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -787,7 +931,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr"/>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Image Name</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Full Image Gen</t>
@@ -798,6 +946,7 @@
           <t>Segment Gen</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -806,11 +955,12 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="C2" t="n">
-        <v>85</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -824,6 +974,7 @@
       <c r="C3" t="n">
         <v>90</v>
       </c>
+      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -832,11 +983,12 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C4" t="n">
         <v>85</v>
       </c>
+      <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -848,98 +1000,162 @@
         <v>90</v>
       </c>
       <c r="C5" t="n">
-        <v>95</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>webflow-full</t>
+          <t>ecommerce</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C6" t="n">
-        <v>90</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Superlist_website</t>
+          <t>webflow-full</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="C7" t="n">
-        <v>90</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Spotify_website</t>
+          <t>complex</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="C8" t="n">
         <v>95</v>
       </c>
+      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>mubasic_website</t>
+          <t>Superlist_website</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C9" t="n">
         <v>90</v>
       </c>
+      <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>overflow_website</t>
+          <t>Spotify_website</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C10" t="n">
-        <v>95</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>RCA_website</t>
+          <t>blog</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="C11" t="n">
-        <v>85</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Crypto_website</t>
+          <t>mubasic_website</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>100</v>
       </c>
       <c r="C12" t="n">
+        <v>95</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>overflow_website</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>95</v>
+      </c>
+      <c r="C13" t="n">
+        <v>90</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>RCA_website</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>30</v>
+      </c>
+      <c r="C14" t="n">
+        <v>70</v>
+      </c>
+      <c r="D14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Crypto_website</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>95</v>
+      </c>
+      <c r="C15" t="n">
         <v>100</v>
+      </c>
+      <c r="D15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="n">
+        <v>95</v>
+      </c>
+      <c r="C16" t="n">
+        <v>95</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Crypto_website</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -953,7 +1169,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -962,7 +1178,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr"/>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Image Name</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Full Image Gen</t>
@@ -973,6 +1193,7 @@
           <t>Segment Gen</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -981,11 +1202,12 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C2" t="n">
-        <v>60</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -994,11 +1216,12 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C3" t="n">
         <v>70</v>
       </c>
+      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1007,11 +1230,12 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C4" t="n">
         <v>75</v>
       </c>
+      <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1020,101 +1244,165 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C5" t="n">
-        <v>70</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>webflow-full</t>
+          <t>ecommerce</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="C6" t="n">
-        <v>70</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Superlist_website</t>
+          <t>webflow-full</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C7" t="n">
-        <v>80</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Spotify_website</t>
+          <t>complex</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="C8" t="n">
-        <v>60</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>mubasic_website</t>
+          <t>Superlist_website</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C9" t="n">
-        <v>75</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>overflow_website</t>
+          <t>Spotify_website</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C10" t="n">
-        <v>80</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>RCA_website</t>
+          <t>blog</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="C11" t="n">
-        <v>60</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>mubasic_website</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>90</v>
+      </c>
+      <c r="C12" t="n">
+        <v>85</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>overflow_website</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>80</v>
+      </c>
+      <c r="C13" t="n">
+        <v>75</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>RCA_website</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>20</v>
+      </c>
+      <c r="C14" t="n">
+        <v>50</v>
+      </c>
+      <c r="D14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>Crypto_website</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>90</v>
-      </c>
-      <c r="C12" t="n">
-        <v>90</v>
+      <c r="B15" t="n">
+        <v>80</v>
+      </c>
+      <c r="C15" t="n">
+        <v>90</v>
+      </c>
+      <c r="D15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="n">
+        <v>80</v>
+      </c>
+      <c r="C16" t="n">
+        <v>85</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Crypto_website</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>